<commit_message>
Cap nhatquy hoach dong
</commit_message>
<xml_diff>
--- a/experiment_results/problem_stats.xlsx
+++ b/experiment_results/problem_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,13 +489,13 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>66.63</v>
+        <v>65.39</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
       </c>
       <c r="H2" t="n">
-        <v>66.63</v>
+        <v>65.39</v>
       </c>
     </row>
     <row r="3">
@@ -508,173 +508,397 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="D3" t="n">
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="E3" t="n">
         <v>50</v>
       </c>
       <c r="F3" t="n">
-        <v>48.16</v>
+        <v>213.44</v>
       </c>
       <c r="G3" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="H3" t="n">
-        <v>48.16</v>
+        <v>3.28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Min</t>
+          <t>Problem 3</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D4" t="n">
-        <v>66.67</v>
+        <v>30</v>
       </c>
       <c r="E4" t="n">
-        <v>50</v>
+        <v>83.33</v>
       </c>
       <c r="F4" t="n">
-        <v>48.16</v>
+        <v>40.06</v>
       </c>
       <c r="G4" t="n">
-        <v>40</v>
+        <v>26.67</v>
       </c>
       <c r="H4" t="n">
-        <v>48.16</v>
+        <v>10.68</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Max</t>
+          <t>Problem 4</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D5" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E5" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F5" t="n">
-        <v>66.63</v>
+        <v>20.83</v>
       </c>
       <c r="G5" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="H5" t="n">
-        <v>66.63</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Mean</t>
+          <t>Problem 5</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D6" t="n">
-        <v>83.33500000000001</v>
+        <v>60</v>
       </c>
       <c r="E6" t="n">
-        <v>75</v>
+        <v>69.44</v>
       </c>
       <c r="F6" t="n">
-        <v>57.395</v>
+        <v>22.32</v>
       </c>
       <c r="G6" t="n">
-        <v>70</v>
+        <v>41.67</v>
       </c>
       <c r="H6" t="n">
-        <v>57.395</v>
+        <v>9.82</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Std</t>
+          <t>Problem 6</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>14.14213562373095</v>
+        <v>60</v>
       </c>
       <c r="D7" t="n">
-        <v>23.56786901694763</v>
+        <v>59.57</v>
       </c>
       <c r="E7" t="n">
-        <v>35.35533905932738</v>
+        <v>74</v>
       </c>
       <c r="F7" t="n">
-        <v>13.06026224851553</v>
+        <v>21.83</v>
       </c>
       <c r="G7" t="n">
-        <v>42.42640687119285</v>
+        <v>44</v>
       </c>
       <c r="H7" t="n">
-        <v>13.06026224851553</v>
+        <v>13.93</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
+          <t>Problem 7</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" t="n">
+        <v>83.33</v>
+      </c>
+      <c r="F8" t="n">
+        <v>10.12</v>
+      </c>
+      <c r="G8" t="n">
+        <v>83.33</v>
+      </c>
+      <c r="H8" t="n">
+        <v>10.12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Problem 8</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>60</v>
+      </c>
+      <c r="D9" t="n">
+        <v>60</v>
+      </c>
+      <c r="E9" t="n">
+        <v>79.55</v>
+      </c>
+      <c r="F9" t="n">
+        <v>15.92</v>
+      </c>
+      <c r="G9" t="n">
+        <v>47.73</v>
+      </c>
+      <c r="H9" t="n">
+        <v>9.550000000000001</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Problem 9</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D10" t="n">
+        <v>100</v>
+      </c>
+      <c r="E10" t="n">
+        <v>80.36</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" t="n">
+        <v>80.36</v>
+      </c>
+      <c r="H10" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Problem 10</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>100</v>
+      </c>
+      <c r="D11" t="n">
+        <v>100</v>
+      </c>
+      <c r="E11" t="n">
+        <v>71.43000000000001</v>
+      </c>
+      <c r="F11" t="n">
+        <v>19.62</v>
+      </c>
+      <c r="G11" t="n">
+        <v>71.43000000000001</v>
+      </c>
+      <c r="H11" t="n">
+        <v>19.62</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Min</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>20</v>
+      </c>
+      <c r="D12" t="n">
+        <v>30</v>
+      </c>
+      <c r="E12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G12" t="n">
+        <v>10</v>
+      </c>
+      <c r="H12" t="n">
+        <v>3.28</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>100</v>
+      </c>
+      <c r="D13" t="n">
+        <v>100</v>
+      </c>
+      <c r="E13" t="n">
+        <v>100</v>
+      </c>
+      <c r="F13" t="n">
+        <v>213.44</v>
+      </c>
+      <c r="G13" t="n">
+        <v>100</v>
+      </c>
+      <c r="H13" t="n">
+        <v>65.39</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Mean</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>72</v>
+      </c>
+      <c r="D14" t="n">
+        <v>72.95699999999999</v>
+      </c>
+      <c r="E14" t="n">
+        <v>76.64400000000001</v>
+      </c>
+      <c r="F14" t="n">
+        <v>43.953</v>
+      </c>
+      <c r="G14" t="n">
+        <v>56.51900000000001</v>
+      </c>
+      <c r="H14" t="n">
+        <v>16.906</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>28.59681411936962</v>
+      </c>
+      <c r="D15" t="n">
+        <v>26.71110133342398</v>
+      </c>
+      <c r="E15" t="n">
+        <v>12.71849501928414</v>
+      </c>
+      <c r="F15" t="n">
+        <v>61.79540850437208</v>
+      </c>
+      <c r="G15" t="n">
+        <v>27.73229262871075</v>
+      </c>
+      <c r="H15" t="n">
+        <v>17.60515088767426</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
           <t>Std / (max - min) %</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>inf</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>inf</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>inf</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>inf</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>inf</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>inf</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>inf</t>
         </is>

</xml_diff>

<commit_message>
Cap nhat 10 bai toan thu nghiem
</commit_message>
<xml_diff>
--- a/experiment_results/problem_stats.xlsx
+++ b/experiment_results/problem_stats.xlsx
@@ -489,13 +489,13 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>65.39</v>
+        <v>66.63</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
       </c>
       <c r="H2" t="n">
-        <v>65.39</v>
+        <v>66.63</v>
       </c>
     </row>
     <row r="3">
@@ -508,22 +508,22 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D3" t="n">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="E3" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F3" t="n">
-        <v>213.44</v>
+        <v>65.84999999999999</v>
       </c>
       <c r="G3" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="H3" t="n">
-        <v>3.28</v>
+        <v>65.84999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -533,25 +533,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>40</v>
+        <v>66.67</v>
       </c>
       <c r="D4" t="n">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="E4" t="n">
-        <v>83.33</v>
+        <v>156.25</v>
       </c>
       <c r="F4" t="n">
-        <v>40.06</v>
+        <v>44.48</v>
       </c>
       <c r="G4" t="n">
-        <v>26.67</v>
+        <v>93.75</v>
       </c>
       <c r="H4" t="n">
-        <v>10.68</v>
+        <v>40.24</v>
       </c>
     </row>
     <row r="5">
@@ -561,25 +561,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>80</v>
+        <v>77.78</v>
       </c>
       <c r="D5" t="n">
-        <v>80</v>
+        <v>80.56</v>
       </c>
       <c r="E5" t="n">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="F5" t="n">
-        <v>20.83</v>
+        <v>22.88</v>
       </c>
       <c r="G5" t="n">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="H5" t="n">
-        <v>16.67</v>
+        <v>19.88</v>
       </c>
     </row>
     <row r="6">
@@ -589,25 +589,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D6" t="n">
-        <v>60</v>
+        <v>95.73</v>
       </c>
       <c r="E6" t="n">
-        <v>69.44</v>
+        <v>85</v>
       </c>
       <c r="F6" t="n">
-        <v>22.32</v>
+        <v>32.72</v>
       </c>
       <c r="G6" t="n">
-        <v>41.67</v>
+        <v>75</v>
       </c>
       <c r="H6" t="n">
-        <v>9.82</v>
+        <v>32.69</v>
       </c>
     </row>
     <row r="7">
@@ -617,25 +617,25 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C7" t="n">
-        <v>60</v>
+        <v>84.62</v>
       </c>
       <c r="D7" t="n">
-        <v>59.57</v>
+        <v>77.84</v>
       </c>
       <c r="E7" t="n">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="F7" t="n">
-        <v>21.83</v>
+        <v>56.52</v>
       </c>
       <c r="G7" t="n">
-        <v>44</v>
+        <v>96.67</v>
       </c>
       <c r="H7" t="n">
-        <v>13.93</v>
+        <v>30.71</v>
       </c>
     </row>
     <row r="8">
@@ -645,25 +645,25 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C8" t="n">
-        <v>100</v>
+        <v>85.70999999999999</v>
       </c>
       <c r="D8" t="n">
-        <v>100</v>
+        <v>78.15000000000001</v>
       </c>
       <c r="E8" t="n">
-        <v>83.33</v>
+        <v>120.49</v>
       </c>
       <c r="F8" t="n">
-        <v>10.12</v>
+        <v>87.09999999999999</v>
       </c>
       <c r="G8" t="n">
-        <v>83.33</v>
+        <v>99.18000000000001</v>
       </c>
       <c r="H8" t="n">
-        <v>10.12</v>
+        <v>35.91</v>
       </c>
     </row>
     <row r="9">
@@ -676,22 +676,22 @@
         <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D9" t="n">
-        <v>60</v>
+        <v>77.52</v>
       </c>
       <c r="E9" t="n">
-        <v>79.55</v>
+        <v>131</v>
       </c>
       <c r="F9" t="n">
-        <v>15.92</v>
+        <v>39.19</v>
       </c>
       <c r="G9" t="n">
-        <v>47.73</v>
+        <v>100</v>
       </c>
       <c r="H9" t="n">
-        <v>9.550000000000001</v>
+        <v>16.54</v>
       </c>
     </row>
     <row r="10">
@@ -701,7 +701,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
         <v>100</v>
@@ -710,16 +710,16 @@
         <v>100</v>
       </c>
       <c r="E10" t="n">
-        <v>80.36</v>
+        <v>85</v>
       </c>
       <c r="F10" t="n">
-        <v>10</v>
+        <v>73.97</v>
       </c>
       <c r="G10" t="n">
-        <v>80.36</v>
+        <v>85</v>
       </c>
       <c r="H10" t="n">
-        <v>10</v>
+        <v>73.97</v>
       </c>
     </row>
     <row r="11">
@@ -729,25 +729,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C11" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="D11" t="n">
-        <v>100</v>
+        <v>77.78</v>
       </c>
       <c r="E11" t="n">
-        <v>71.43000000000001</v>
+        <v>180</v>
       </c>
       <c r="F11" t="n">
-        <v>19.62</v>
+        <v>183.94</v>
       </c>
       <c r="G11" t="n">
-        <v>71.43000000000001</v>
+        <v>100</v>
       </c>
       <c r="H11" t="n">
-        <v>19.62</v>
+        <v>88.94</v>
       </c>
     </row>
     <row r="12">
@@ -757,25 +757,25 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
         <v>20</v>
       </c>
       <c r="D12" t="n">
-        <v>30</v>
+        <v>77.52</v>
       </c>
       <c r="E12" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F12" t="n">
-        <v>10</v>
+        <v>22.88</v>
       </c>
       <c r="G12" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="H12" t="n">
-        <v>3.28</v>
+        <v>16.54</v>
       </c>
     </row>
     <row r="13">
@@ -785,7 +785,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C13" t="n">
         <v>100</v>
@@ -794,16 +794,16 @@
         <v>100</v>
       </c>
       <c r="E13" t="n">
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="F13" t="n">
-        <v>213.44</v>
+        <v>183.94</v>
       </c>
       <c r="G13" t="n">
         <v>100</v>
       </c>
       <c r="H13" t="n">
-        <v>65.39</v>
+        <v>88.94</v>
       </c>
     </row>
     <row r="14">
@@ -813,25 +813,25 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>5</v>
+        <v>8.9</v>
       </c>
       <c r="C14" t="n">
-        <v>72</v>
+        <v>79.47800000000001</v>
       </c>
       <c r="D14" t="n">
-        <v>72.95699999999999</v>
+        <v>86.758</v>
       </c>
       <c r="E14" t="n">
-        <v>76.64400000000001</v>
+        <v>114.574</v>
       </c>
       <c r="F14" t="n">
-        <v>43.953</v>
+        <v>67.328</v>
       </c>
       <c r="G14" t="n">
-        <v>56.51900000000001</v>
+        <v>90.35999999999999</v>
       </c>
       <c r="H14" t="n">
-        <v>16.906</v>
+        <v>47.136</v>
       </c>
     </row>
     <row r="15">
@@ -841,25 +841,25 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>5.466056876558985</v>
       </c>
       <c r="C15" t="n">
-        <v>28.59681411936962</v>
+        <v>24.11509660864838</v>
       </c>
       <c r="D15" t="n">
-        <v>26.71110133342398</v>
+        <v>10.59458855579898</v>
       </c>
       <c r="E15" t="n">
-        <v>12.71849501928414</v>
+        <v>33.9654854881311</v>
       </c>
       <c r="F15" t="n">
-        <v>61.79540850437208</v>
+        <v>45.50947124866794</v>
       </c>
       <c r="G15" t="n">
-        <v>27.73229262871075</v>
+        <v>11.19289357881449</v>
       </c>
       <c r="H15" t="n">
-        <v>17.60515088767426</v>
+        <v>24.78563840434841</v>
       </c>
     </row>
     <row r="16">
@@ -868,40 +868,26 @@
           <t>Std / (max - min) %</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="B16" t="n">
+        <v>30.36698264754992</v>
+      </c>
+      <c r="C16" t="n">
+        <v>30.14387076081047</v>
+      </c>
+      <c r="D16" t="n">
+        <v>47.12895265035132</v>
+      </c>
+      <c r="E16" t="n">
+        <v>30.87771408011918</v>
+      </c>
+      <c r="F16" t="n">
+        <v>28.25622205927477</v>
+      </c>
+      <c r="G16" t="n">
+        <v>37.30964526271497</v>
+      </c>
+      <c r="H16" t="n">
+        <v>34.23430718832653</v>
       </c>
     </row>
   </sheetData>

</xml_diff>